<commit_message>
Add Buff and other stuff
</commit_message>
<xml_diff>
--- a/My project/Luban/Config/Datas/CardInfo.xlsx
+++ b/My project/Luban/Config/Datas/CardInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lofnh\Documents\GitHub\Draconia\My project\Luban\Config\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0334A8D-9D3E-40F0-937E-1B4127362A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E5DB51-F35E-456C-B852-DD9927EEFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="8730" windowWidth="28800" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="9675" windowWidth="28800" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>##</t>
   </si>
@@ -133,10 +133,93 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>造成80%物理伤害，将敌方单位挪动一个单位，造成该敌方单位重心不稳，使其硬直增加。</t>
-  </si>
-  <si>
-    <t>清除一名友方单位的后摇，提升自身速度20%。（2s）</t>
+    <t>技能对象</t>
+  </si>
+  <si>
+    <t>SkillTarget</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillTargetType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SingleEnemy</t>
+  </si>
+  <si>
+    <t>SingleEnemy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AroundSelf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SingleAlly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成100%物理伤害,回复一点行动力,{虚幻}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动一格位置,{虚幻}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加物理防御和魔法抗性20%，减少受击硬直20%,{虚幻}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BelongedCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从属英雄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int#ref=TbPlayerInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Properties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Virtual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list#sep=|,EnumCardProperty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>Flash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -162,63 +245,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>技能卡（</t>
+      <t>技能卡，它具有{虚幻}，{闪回}</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>闪回</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <t>技能对象</t>
-  </si>
-  <si>
-    <t>SkillTarget</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillTargetType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SingleEnemy</t>
-  </si>
-  <si>
-    <t>SingleEnemy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>防御</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立即开始一名友方单位的回合，提升自身速度20%直到下个回合开始。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -245,54 +277,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>技能卡（</t>
+      <t>技能卡，它具有{虚幻}，{闪回}</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>闪回</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）。</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AroundSelf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对敌方单位攻击，造成120%物理伤害，使用后获得一层【清风】（清风：增加攻击力20%，最高可叠加3层。且3层后获得所有伤害百分之50真实伤害buff）。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>造成100%物理伤害,回复一点行动力,虚幻</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动一格位置,虚幻</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>增加物理防御和魔法抗性20%，减少受击硬直20%,虚幻</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SingleAlly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成80%物理伤害，{推}目标一格，造成该敌方单位{重心不稳}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成120%物理伤害，使用后获得一层{清风}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -630,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -641,7 +635,7 @@
     <col min="4" max="4" width="60.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,10 +667,16 @@
         <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -708,10 +708,16 @@
         <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,19 +749,25 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -773,19 +785,25 @@
         <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="L4">
+        <v>10001</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -804,19 +822,25 @@
       </c>
       <c r="J5" s="1"/>
       <c r="K5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="L5">
+        <v>10001</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>102</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -835,10 +859,16 @@
       </c>
       <c r="J6" s="1"/>
       <c r="K6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="L6">
+        <v>10001</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>103</v>
@@ -847,7 +877,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -866,10 +896,13 @@
       </c>
       <c r="J7" s="1"/>
       <c r="K7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="L7">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>104</v>
@@ -878,7 +911,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -897,10 +930,16 @@
       </c>
       <c r="J8" s="1"/>
       <c r="K8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="L8">
+        <v>10001</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>105</v>
       </c>
@@ -908,7 +947,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -927,10 +966,13 @@
       </c>
       <c r="J9" s="1"/>
       <c r="K9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="L9">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>106</v>
       </c>
@@ -938,7 +980,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -957,10 +999,13 @@
       </c>
       <c r="J10" s="1"/>
       <c r="K10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="L10">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>107</v>
       </c>
@@ -968,7 +1013,7 @@
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -987,10 +1032,16 @@
       </c>
       <c r="J11" s="1"/>
       <c r="K11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="L11">
+        <v>10001</v>
+      </c>
+      <c r="M11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1001,7 +1052,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1012,7 +1063,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1023,7 +1074,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Doc Change/ Move Animation and Card Animation Change
1.更改了显示逻辑，
2.解决了Intention被遮挡的问题
3,移动现在变得更加顺滑
4.卡牌逻辑更新，UI更新一部分

接下来：弃牌堆/抽牌堆 UI展示
牌堆抽取逻辑
廷巴克图卡牌
敌人攻击逻辑/策略更新
</commit_message>
<xml_diff>
--- a/My project/Luban/Config/Datas/CardInfo.xlsx
+++ b/My project/Luban/Config/Datas/CardInfo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lofnh\Documents\GitHub\Draconia\My project\Luban\Config\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E5DB51-F35E-456C-B852-DD9927EEFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0BAAD9-0F78-45FB-8D94-6A7D4297F254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="9675" windowWidth="28800" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26775" yWindow="9360" windowWidth="28740" windowHeight="9915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Zhouzhou" sheetId="1" r:id="rId1"/>
+    <sheet name="Timbuktu" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="64">
   <si>
     <t>##</t>
   </si>
@@ -175,18 +176,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>造成100%物理伤害,回复一点行动力,{虚幻}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动一格位置,{虚幻}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>增加物理防御和魔法抗性20%，减少受击硬直20%,{虚幻}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BelongedCharacter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -195,10 +184,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>int#ref=TbPlayerInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Properties</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -215,78 +200,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Flash</t>
-  </si>
-  <si>
-    <t>Flash</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>造成190%物理伤害，随机获得一张</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>周周</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>技能卡，它具有{虚幻}，{闪回}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>立即开始一名友方单位的回合，提升自身速度20%直到下个回合开始。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>对下一次的伤害必定闪避，闪避成功随机获得一张</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>周周</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>技能卡，它具有{虚幻}，{闪回}</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>造成80%物理伤害，{推}目标一格，造成该敌方单位{重心不稳}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>造成120%物理伤害，使用后获得一层{清风}</t>
+    <t>造成2伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得2临时护甲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成3点伤害，若该单位处于危险区则再攻击一次。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成2点伤害，并给予所有在危险区的敌方单位造成等量破甲。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（姿态）增加敌方危险区至4。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使一名友方单位-2费用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（姿态）触发避柳时获得一张免费的基础牌，一次行动只能触发一次。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string#ref=TbPlayerInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhouzhou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timbuktu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叠甲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成5伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成3伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得3临时护甲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>##</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -294,7 +276,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,15 +286,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -626,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -670,10 +643,10 @@
         <v>31</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
@@ -711,10 +684,10 @@
         <v>30</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -752,10 +725,10 @@
         <v>29</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -767,16 +740,16 @@
         <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -787,11 +760,11 @@
       <c r="K4" t="s">
         <v>33</v>
       </c>
-      <c r="L4">
-        <v>10001</v>
+      <c r="L4" t="s">
+        <v>55</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -803,7 +776,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -812,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1">
         <v>3</v>
@@ -824,11 +797,11 @@
       <c r="K5" t="s">
         <v>38</v>
       </c>
-      <c r="L5">
-        <v>10001</v>
+      <c r="L5" t="s">
+        <v>55</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -840,16 +813,16 @@
         <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -861,11 +834,11 @@
       <c r="K6" t="s">
         <v>34</v>
       </c>
-      <c r="L6">
-        <v>10001</v>
+      <c r="L6" t="s">
+        <v>55</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -877,16 +850,16 @@
         <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <v>3</v>
@@ -898,12 +871,14 @@
       <c r="K7" t="s">
         <v>32</v>
       </c>
-      <c r="L7">
-        <v>10001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+      <c r="L7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="B8" s="1">
         <v>104</v>
       </c>
@@ -911,16 +886,16 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -932,14 +907,15 @@
       <c r="K8" t="s">
         <v>34</v>
       </c>
-      <c r="L8">
-        <v>10001</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="L8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
       <c r="B9" s="1">
         <v>105</v>
       </c>
@@ -947,16 +923,16 @@
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="F9" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
         <v>4</v>
@@ -968,11 +944,14 @@
       <c r="K9" t="s">
         <v>32</v>
       </c>
-      <c r="L9">
-        <v>10001</v>
+      <c r="L9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
       <c r="B10" s="1">
         <v>106</v>
       </c>
@@ -986,10 +965,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -1001,8 +980,8 @@
       <c r="K10" t="s">
         <v>39</v>
       </c>
-      <c r="L10">
-        <v>10001</v>
+      <c r="L10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1019,10 +998,534 @@
         <v>2</v>
       </c>
       <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4</v>
+      </c>
+      <c r="I11" s="1">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <v>108</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>109</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
+        <v>110</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1D3614-7E2B-4457-A75F-23F93B69E534}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="60.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
+        <v>201</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6">
+        <v>202</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1">
+        <v>203</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>8</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8">
+        <v>204</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>205</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
+        <v>11</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>206</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>207</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
       <c r="G11" s="1">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
         <v>4</v>
@@ -1034,11 +1537,8 @@
       <c r="K11" t="s">
         <v>32</v>
       </c>
-      <c r="L11">
-        <v>10001</v>
-      </c>
-      <c r="M11" t="s">
-        <v>50</v>
+      <c r="L11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1081,6 +1581,5 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>